<commit_message>
Commit correcciones diseño Prototipo 1
</commit_message>
<xml_diff>
--- a/2. SRS/Anexos/4. Validación de requisitos.xlsx
+++ b/2. SRS/Anexos/4. Validación de requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Chafloque\Desktop\Javeriana\10. Decimo Semestre\Ingeniería de Software\Smart Closet\Smart-Closet\2. SRS\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA917A06-5BFB-457C-ABDC-DC3136092180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0201DC01-2757-4717-83C9-F9A957352993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,31 +258,26 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1041,7 +1036,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -1088,7 +1083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -1182,7 +1177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
@@ -1229,7 +1224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>43</v>
       </c>
@@ -1276,7 +1271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1323,7 +1318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
@@ -1370,7 +1365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
@@ -1417,7 +1412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>51</v>
       </c>

</xml_diff>